<commit_message>
add rate limit code
</commit_message>
<xml_diff>
--- a/product_info.xlsx
+++ b/product_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="14">
   <si>
     <t>title</t>
   </si>
@@ -51,31 +51,16 @@
     <t>Snowboard</t>
   </si>
   <si>
-    <t>Burton Custom</t>
+    <t>sku</t>
   </si>
   <si>
-    <t>&lt;strong&gt;Good custom!&lt;/strong&gt;</t>
+    <t>sku_title</t>
   </si>
   <si>
-    <t>Apna start</t>
+    <t>snowboard</t>
   </si>
   <si>
-    <t>Burton-custom</t>
-  </si>
-  <si>
-    <t>custom</t>
-  </si>
-  <si>
-    <t>Test Product</t>
-  </si>
-  <si>
-    <t>&lt;strong&gt;Test Product!&lt;/strong&gt;</t>
-  </si>
-  <si>
-    <t>test-product</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>snow</t>
   </si>
 </sst>
 </file>
@@ -882,22 +867,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -913,8 +900,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -930,39 +923,908 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rate limit code added
</commit_message>
<xml_diff>
--- a/product_info.xlsx
+++ b/product_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="182">
   <si>
     <t>title</t>
   </si>
@@ -61,6 +61,510 @@
   </si>
   <si>
     <t>snow</t>
+  </si>
+  <si>
+    <t>snow20</t>
+  </si>
+  <si>
+    <t>snow1</t>
+  </si>
+  <si>
+    <t>snow2</t>
+  </si>
+  <si>
+    <t>snowboard1</t>
+  </si>
+  <si>
+    <t>snowboard19</t>
+  </si>
+  <si>
+    <t>snowboard20</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Good snowboard! 20&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Good snowboard! 1&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>snowboard21</t>
+  </si>
+  <si>
+    <t>snow21</t>
+  </si>
+  <si>
+    <t>snowboard22</t>
+  </si>
+  <si>
+    <t>snow22</t>
+  </si>
+  <si>
+    <t>snowboard23</t>
+  </si>
+  <si>
+    <t>snow23</t>
+  </si>
+  <si>
+    <t>snowboard24</t>
+  </si>
+  <si>
+    <t>snow24</t>
+  </si>
+  <si>
+    <t>snowboard25</t>
+  </si>
+  <si>
+    <t>snow25</t>
+  </si>
+  <si>
+    <t>snowboard26</t>
+  </si>
+  <si>
+    <t>snow26</t>
+  </si>
+  <si>
+    <t>snowboard27</t>
+  </si>
+  <si>
+    <t>snow27</t>
+  </si>
+  <si>
+    <t>snowboard28</t>
+  </si>
+  <si>
+    <t>snow28</t>
+  </si>
+  <si>
+    <t>snowboard29</t>
+  </si>
+  <si>
+    <t>snow29</t>
+  </si>
+  <si>
+    <t>snowboard30</t>
+  </si>
+  <si>
+    <t>snow30</t>
+  </si>
+  <si>
+    <t>snowboard31</t>
+  </si>
+  <si>
+    <t>snow31</t>
+  </si>
+  <si>
+    <t>snowboard32</t>
+  </si>
+  <si>
+    <t>snow32</t>
+  </si>
+  <si>
+    <t>snowboard33</t>
+  </si>
+  <si>
+    <t>snow33</t>
+  </si>
+  <si>
+    <t>snowboard34</t>
+  </si>
+  <si>
+    <t>snow34</t>
+  </si>
+  <si>
+    <t>snowboard35</t>
+  </si>
+  <si>
+    <t>snow35</t>
+  </si>
+  <si>
+    <t>snowboard36</t>
+  </si>
+  <si>
+    <t>snow36</t>
+  </si>
+  <si>
+    <t>snowboard37</t>
+  </si>
+  <si>
+    <t>snow37</t>
+  </si>
+  <si>
+    <t>snowboard38</t>
+  </si>
+  <si>
+    <t>snow38</t>
+  </si>
+  <si>
+    <t>snowboard39</t>
+  </si>
+  <si>
+    <t>snow39</t>
+  </si>
+  <si>
+    <t>snowboard40</t>
+  </si>
+  <si>
+    <t>snow40</t>
+  </si>
+  <si>
+    <t>snowboard41</t>
+  </si>
+  <si>
+    <t>snow41</t>
+  </si>
+  <si>
+    <t>snowboard42</t>
+  </si>
+  <si>
+    <t>snow42</t>
+  </si>
+  <si>
+    <t>snowboard43</t>
+  </si>
+  <si>
+    <t>snow43</t>
+  </si>
+  <si>
+    <t>snowboard44</t>
+  </si>
+  <si>
+    <t>snow44</t>
+  </si>
+  <si>
+    <t>snowboard45</t>
+  </si>
+  <si>
+    <t>snow45</t>
+  </si>
+  <si>
+    <t>snowboard46</t>
+  </si>
+  <si>
+    <t>snow46</t>
+  </si>
+  <si>
+    <t>snowboard47</t>
+  </si>
+  <si>
+    <t>snow47</t>
+  </si>
+  <si>
+    <t>snowboard48</t>
+  </si>
+  <si>
+    <t>snow48</t>
+  </si>
+  <si>
+    <t>snowboard49</t>
+  </si>
+  <si>
+    <t>snow49</t>
+  </si>
+  <si>
+    <t>snowboard50</t>
+  </si>
+  <si>
+    <t>snow50</t>
+  </si>
+  <si>
+    <t>snowboard51</t>
+  </si>
+  <si>
+    <t>snow51</t>
+  </si>
+  <si>
+    <t>snowboard52</t>
+  </si>
+  <si>
+    <t>snow52</t>
+  </si>
+  <si>
+    <t>snowboard53</t>
+  </si>
+  <si>
+    <t>snow53</t>
+  </si>
+  <si>
+    <t>snowboard54</t>
+  </si>
+  <si>
+    <t>snow54</t>
+  </si>
+  <si>
+    <t>snowboard55</t>
+  </si>
+  <si>
+    <t>snow55</t>
+  </si>
+  <si>
+    <t>snowboard56</t>
+  </si>
+  <si>
+    <t>snow56</t>
+  </si>
+  <si>
+    <t>snowboard57</t>
+  </si>
+  <si>
+    <t>snow57</t>
+  </si>
+  <si>
+    <t>snowboard58</t>
+  </si>
+  <si>
+    <t>snow58</t>
+  </si>
+  <si>
+    <t>snowboard59</t>
+  </si>
+  <si>
+    <t>snow59</t>
+  </si>
+  <si>
+    <t>snowboard60</t>
+  </si>
+  <si>
+    <t>snow60</t>
+  </si>
+  <si>
+    <t>snowboard61</t>
+  </si>
+  <si>
+    <t>snow61</t>
+  </si>
+  <si>
+    <t>snowboard62</t>
+  </si>
+  <si>
+    <t>snow62</t>
+  </si>
+  <si>
+    <t>snowboard63</t>
+  </si>
+  <si>
+    <t>snow63</t>
+  </si>
+  <si>
+    <t>snowboard64</t>
+  </si>
+  <si>
+    <t>snow64</t>
+  </si>
+  <si>
+    <t>snowboard65</t>
+  </si>
+  <si>
+    <t>snow65</t>
+  </si>
+  <si>
+    <t>snowboard66</t>
+  </si>
+  <si>
+    <t>snow66</t>
+  </si>
+  <si>
+    <t>snowboard67</t>
+  </si>
+  <si>
+    <t>snow67</t>
+  </si>
+  <si>
+    <t>snowboard68</t>
+  </si>
+  <si>
+    <t>snow68</t>
+  </si>
+  <si>
+    <t>snowboard69</t>
+  </si>
+  <si>
+    <t>snow69</t>
+  </si>
+  <si>
+    <t>snowboard70</t>
+  </si>
+  <si>
+    <t>snow70</t>
+  </si>
+  <si>
+    <t>snowboard71</t>
+  </si>
+  <si>
+    <t>snow71</t>
+  </si>
+  <si>
+    <t>snowboard72</t>
+  </si>
+  <si>
+    <t>snow72</t>
+  </si>
+  <si>
+    <t>snowboard73</t>
+  </si>
+  <si>
+    <t>snow73</t>
+  </si>
+  <si>
+    <t>snowboard74</t>
+  </si>
+  <si>
+    <t>snow74</t>
+  </si>
+  <si>
+    <t>snowboard75</t>
+  </si>
+  <si>
+    <t>snow75</t>
+  </si>
+  <si>
+    <t>snowboard76</t>
+  </si>
+  <si>
+    <t>snow76</t>
+  </si>
+  <si>
+    <t>snowboard77</t>
+  </si>
+  <si>
+    <t>snow77</t>
+  </si>
+  <si>
+    <t>snowboard78</t>
+  </si>
+  <si>
+    <t>snow78</t>
+  </si>
+  <si>
+    <t>snowboard79</t>
+  </si>
+  <si>
+    <t>snow79</t>
+  </si>
+  <si>
+    <t>snowboard80</t>
+  </si>
+  <si>
+    <t>snow80</t>
+  </si>
+  <si>
+    <t>snowboard81</t>
+  </si>
+  <si>
+    <t>snow81</t>
+  </si>
+  <si>
+    <t>snowboard82</t>
+  </si>
+  <si>
+    <t>snow82</t>
+  </si>
+  <si>
+    <t>snowboard83</t>
+  </si>
+  <si>
+    <t>snow83</t>
+  </si>
+  <si>
+    <t>snowboard84</t>
+  </si>
+  <si>
+    <t>snow84</t>
+  </si>
+  <si>
+    <t>snowboard85</t>
+  </si>
+  <si>
+    <t>snow85</t>
+  </si>
+  <si>
+    <t>snowboard86</t>
+  </si>
+  <si>
+    <t>snow86</t>
+  </si>
+  <si>
+    <t>snowboard87</t>
+  </si>
+  <si>
+    <t>snow87</t>
+  </si>
+  <si>
+    <t>snowboard88</t>
+  </si>
+  <si>
+    <t>snow88</t>
+  </si>
+  <si>
+    <t>snowboard89</t>
+  </si>
+  <si>
+    <t>snow89</t>
+  </si>
+  <si>
+    <t>snowboard90</t>
+  </si>
+  <si>
+    <t>snow90</t>
+  </si>
+  <si>
+    <t>snowboard91</t>
+  </si>
+  <si>
+    <t>snow91</t>
+  </si>
+  <si>
+    <t>snowboard92</t>
+  </si>
+  <si>
+    <t>snow92</t>
+  </si>
+  <si>
+    <t>snowboard93</t>
+  </si>
+  <si>
+    <t>snow93</t>
+  </si>
+  <si>
+    <t>snowboard94</t>
+  </si>
+  <si>
+    <t>snow94</t>
+  </si>
+  <si>
+    <t>snowboard95</t>
+  </si>
+  <si>
+    <t>snow95</t>
+  </si>
+  <si>
+    <t>snowboard96</t>
+  </si>
+  <si>
+    <t>snow96</t>
+  </si>
+  <si>
+    <t>snowboard97</t>
+  </si>
+  <si>
+    <t>snow97</t>
+  </si>
+  <si>
+    <t>snowboard98</t>
+  </si>
+  <si>
+    <t>snow98</t>
+  </si>
+  <si>
+    <t>snowboard99</t>
+  </si>
+  <si>
+    <t>snow99</t>
+  </si>
+  <si>
+    <t>snowboard100</t>
+  </si>
+  <si>
+    <t>snow100</t>
   </si>
 </sst>
 </file>
@@ -867,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="J97" sqref="J97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +1416,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -924,10 +1428,10 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -950,7 +1454,7 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1338,7 +1842,7 @@
         <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s">
         <v>13</v>
@@ -1349,7 +1853,7 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -1361,10 +1865,10 @@
         <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1372,7 +1876,7 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1384,10 +1888,10 @@
         <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1395,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1407,10 +1911,10 @@
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1418,7 +1922,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -1430,10 +1934,10 @@
         <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1441,7 +1945,7 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -1453,10 +1957,10 @@
         <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1464,7 +1968,7 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -1476,10 +1980,10 @@
         <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1487,7 +1991,7 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
@@ -1499,10 +2003,10 @@
         <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1510,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
         <v>7</v>
@@ -1522,10 +2026,10 @@
         <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1533,7 +2037,7 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
         <v>7</v>
@@ -1545,10 +2049,10 @@
         <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G29" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1556,7 +2060,7 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -1568,10 +2072,10 @@
         <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1579,7 +2083,7 @@
         <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1591,10 +2095,10 @@
         <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G31" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1602,7 +2106,7 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1614,10 +2118,10 @@
         <v>9</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G32" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1625,7 +2129,7 @@
         <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1637,10 +2141,10 @@
         <v>9</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1648,7 +2152,7 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -1660,10 +2164,10 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="G34" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1671,7 +2175,7 @@
         <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1683,10 +2187,10 @@
         <v>9</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G35" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1694,7 +2198,7 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -1706,10 +2210,10 @@
         <v>9</v>
       </c>
       <c r="F36" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1717,7 +2221,7 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1729,10 +2233,10 @@
         <v>9</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1740,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -1752,10 +2256,10 @@
         <v>9</v>
       </c>
       <c r="F38" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="G38" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,7 +2267,7 @@
         <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1775,10 +2279,10 @@
         <v>9</v>
       </c>
       <c r="F39" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1786,7 +2290,7 @@
         <v>5</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1798,10 +2302,10 @@
         <v>9</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1809,7 +2313,7 @@
         <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -1821,10 +2325,1390 @@
         <v>9</v>
       </c>
       <c r="F41" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>13</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" t="s">
+        <v>66</v>
+      </c>
+      <c r="G44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>20</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" t="s">
+        <v>68</v>
+      </c>
+      <c r="G45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G46" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G47" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" t="s">
+        <v>76</v>
+      </c>
+      <c r="G49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" t="s">
+        <v>78</v>
+      </c>
+      <c r="G50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>80</v>
+      </c>
+      <c r="G51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>84</v>
+      </c>
+      <c r="G53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" t="s">
+        <v>86</v>
+      </c>
+      <c r="G54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" t="s">
+        <v>88</v>
+      </c>
+      <c r="G55" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" t="s">
+        <v>90</v>
+      </c>
+      <c r="G56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" t="s">
+        <v>92</v>
+      </c>
+      <c r="G57" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" t="s">
+        <v>94</v>
+      </c>
+      <c r="G58" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" t="s">
+        <v>96</v>
+      </c>
+      <c r="G59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" t="s">
+        <v>98</v>
+      </c>
+      <c r="G60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>102</v>
+      </c>
+      <c r="G62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>5</v>
+      </c>
+      <c r="B63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>104</v>
+      </c>
+      <c r="G63" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" t="s">
+        <v>20</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" t="s">
+        <v>106</v>
+      </c>
+      <c r="G64" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" t="s">
+        <v>108</v>
+      </c>
+      <c r="G65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" t="s">
+        <v>110</v>
+      </c>
+      <c r="G66" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" t="s">
+        <v>112</v>
+      </c>
+      <c r="G67" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" t="s">
+        <v>114</v>
+      </c>
+      <c r="G68" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" t="s">
+        <v>116</v>
+      </c>
+      <c r="G69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>9</v>
+      </c>
+      <c r="F70" t="s">
+        <v>118</v>
+      </c>
+      <c r="G70" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" t="s">
+        <v>9</v>
+      </c>
+      <c r="F71" t="s">
+        <v>120</v>
+      </c>
+      <c r="G71" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>9</v>
+      </c>
+      <c r="F72" t="s">
+        <v>122</v>
+      </c>
+      <c r="G72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" t="s">
+        <v>9</v>
+      </c>
+      <c r="F73" t="s">
+        <v>124</v>
+      </c>
+      <c r="G73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" t="s">
+        <v>126</v>
+      </c>
+      <c r="G74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" t="s">
+        <v>20</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" t="s">
+        <v>128</v>
+      </c>
+      <c r="G75" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G76" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>8</v>
+      </c>
+      <c r="E77" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" t="s">
+        <v>132</v>
+      </c>
+      <c r="G77" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" t="s">
+        <v>134</v>
+      </c>
+      <c r="G78" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" t="s">
+        <v>9</v>
+      </c>
+      <c r="F79" t="s">
+        <v>136</v>
+      </c>
+      <c r="G79" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" t="s">
+        <v>138</v>
+      </c>
+      <c r="G80" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" t="s">
+        <v>140</v>
+      </c>
+      <c r="G81" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" t="s">
+        <v>142</v>
+      </c>
+      <c r="G82" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" t="s">
+        <v>20</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" t="s">
+        <v>9</v>
+      </c>
+      <c r="F83" t="s">
+        <v>144</v>
+      </c>
+      <c r="G83" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" t="s">
+        <v>20</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" t="s">
+        <v>146</v>
+      </c>
+      <c r="G84" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" t="s">
+        <v>148</v>
+      </c>
+      <c r="G85" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>150</v>
+      </c>
+      <c r="G86" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" t="s">
+        <v>152</v>
+      </c>
+      <c r="G87" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" t="s">
+        <v>154</v>
+      </c>
+      <c r="G88" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" t="s">
+        <v>156</v>
+      </c>
+      <c r="G89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" t="s">
+        <v>9</v>
+      </c>
+      <c r="F90" t="s">
+        <v>158</v>
+      </c>
+      <c r="G90" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" t="s">
+        <v>160</v>
+      </c>
+      <c r="G91" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" t="s">
+        <v>20</v>
+      </c>
+      <c r="C92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" t="s">
+        <v>162</v>
+      </c>
+      <c r="G92" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" t="s">
+        <v>164</v>
+      </c>
+      <c r="G93" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>166</v>
+      </c>
+      <c r="G94" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" t="s">
+        <v>7</v>
+      </c>
+      <c r="D95" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" t="s">
+        <v>168</v>
+      </c>
+      <c r="G95" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" t="s">
+        <v>170</v>
+      </c>
+      <c r="G96" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>9</v>
+      </c>
+      <c r="F97" t="s">
+        <v>172</v>
+      </c>
+      <c r="G97" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" t="s">
+        <v>174</v>
+      </c>
+      <c r="G98" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" t="s">
+        <v>176</v>
+      </c>
+      <c r="G99" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>178</v>
+      </c>
+      <c r="G100" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" t="s">
+        <v>180</v>
+      </c>
+      <c r="G101" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>